<commit_message>
Got google sheet BOM processing operational
</commit_message>
<xml_diff>
--- a/src/ASSY REV.xlsx
+++ b/src/ASSY REV.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pumpkin\Altium_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pumpkin\Altium_docs\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ASSY REV" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="59">
   <si>
     <t>Encoding:</t>
   </si>
@@ -891,7 +891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -1513,7 +1513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -4334,7 +4334,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4622,41 +4622,31 @@
       <c r="B26" t="s">
         <v>56</v>
       </c>
-      <c r="C26" t="s">
-        <v>57</v>
-      </c>
+      <c r="C26"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>56</v>
       </c>
-      <c r="C27" t="s">
-        <v>57</v>
-      </c>
+      <c r="C27"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C28" t="s">
-        <v>57</v>
-      </c>
+      <c r="C28"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C29" t="s">
-        <v>57</v>
-      </c>
+      <c r="C29"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C30" t="s">
-        <v>57</v>
-      </c>
+      <c r="C30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>